<commit_message>
regression param lossy vs lossless test
</commit_message>
<xml_diff>
--- a/experiment/reg_param/result.xlsx
+++ b/experiment/reg_param/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzhao/code/meta_compressor/experiment/reg_param/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9011CE4-FAF1-284D-A20E-3C7319240257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307039CD-A4FC-7A49-9D59-C4B30ACB5C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0C42B66A-AB11-6046-9434-D877C62AFB22}"/>
   </bookViews>
@@ -16142,12 +16142,12 @@
   <dimension ref="A1:G507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
+    <col min="1" max="1" width="64.33203125" customWidth="1"/>
     <col min="4" max="4" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>